<commit_message>
improves main level func
</commit_message>
<xml_diff>
--- a/Documents/ToDo.xlsx
+++ b/Documents/ToDo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro\Desktop\PlayGround\Games\FirstPlatformer\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A042F6F-FE47-439E-AA2D-657CD19AB891}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{315474F5-37AF-4464-917E-B7153CE87CBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37440" yWindow="4650" windowWidth="21600" windowHeight="11100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Design</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>Work On Enemy</t>
+  </si>
+  <si>
+    <t>"="</t>
   </si>
 </sst>
 </file>
@@ -83,9 +86,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -366,10 +372,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B4:E6"/>
+  <dimension ref="B4:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -378,7 +384,7 @@
     <col min="5" max="5" width="20.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -386,15 +392,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>1</v>
       </c>
       <c r="E5" t="s">
         <v>3</v>
       </c>
+      <c r="F5" s="2" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="E6" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
adds func to enemy
</commit_message>
<xml_diff>
--- a/Documents/ToDo.xlsx
+++ b/Documents/ToDo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro\Desktop\PlayGround\Games\FirstPlatformer\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4325B5FF-7A96-4D61-B89F-AC196C70E4BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04E8832C-2DC6-414C-B0DB-6598CEBA0677}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29760" yWindow="960" windowWidth="38700" windowHeight="15285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,9 +39,6 @@
     <t>Work on sound</t>
   </si>
   <si>
-    <t>Work on orbs</t>
-  </si>
-  <si>
     <t>Work on projectiles/fire</t>
   </si>
   <si>
@@ -52,6 +49,9 @@
   </si>
   <si>
     <t>give a slide to the player</t>
+  </si>
+  <si>
+    <t>Work On Menu</t>
   </si>
 </sst>
 </file>
@@ -384,7 +384,7 @@
   <dimension ref="B4:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -412,25 +412,25 @@
         <v>3</v>
       </c>
       <c r="E6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
improves slide and burning_fire
</commit_message>
<xml_diff>
--- a/Documents/ToDo.xlsx
+++ b/Documents/ToDo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro\Desktop\PlayGround\Games\FirstPlatformer\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04E8832C-2DC6-414C-B0DB-6598CEBA0677}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{882C584C-2DD7-4340-9070-1AE21456E1DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29760" yWindow="960" windowWidth="38700" windowHeight="15285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Design</t>
   </si>
@@ -52,6 +52,27 @@
   </si>
   <si>
     <t>Work On Menu</t>
+  </si>
+  <si>
+    <t>Phase 1:</t>
+  </si>
+  <si>
+    <t>Modify Player Mov Speed</t>
+  </si>
+  <si>
+    <t>Change From fire to energy Fields</t>
+  </si>
+  <si>
+    <t>Change Behavior of the orbs</t>
+  </si>
+  <si>
+    <t>Change The points system</t>
+  </si>
+  <si>
+    <t>Player will have to fill the score bar to advance to phase 2</t>
+  </si>
+  <si>
+    <t>Define Phase 2</t>
   </si>
 </sst>
 </file>
@@ -381,15 +402,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B4:F9"/>
+  <dimension ref="B4:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -433,6 +455,39 @@
         <v>5</v>
       </c>
     </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
adds strike zone behaviour
</commit_message>
<xml_diff>
--- a/Documents/ToDo.xlsx
+++ b/Documents/ToDo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro\Desktop\PlayGround\Games\FirstPlatformer\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{882C584C-2DD7-4340-9070-1AE21456E1DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E666C5F-43D2-4D4D-BCA8-C67381082636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Design</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>Define Phase 2</t>
+  </si>
+  <si>
+    <t>TO BE DECIDED: Spawn Position, random or markers?</t>
   </si>
 </sst>
 </file>
@@ -404,14 +407,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B4:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="28.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="51.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -469,6 +472,9 @@
       <c r="B14" t="s">
         <v>11</v>
       </c>
+      <c r="C14" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B15" t="s">

</xml_diff>

<commit_message>
adds FSM to enemy
</commit_message>
<xml_diff>
--- a/Documents/ToDo.xlsx
+++ b/Documents/ToDo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro\Desktop\PlayGround\Games\FirstPlatformer\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E666C5F-43D2-4D4D-BCA8-C67381082636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9548889B-0CEF-4B1A-86D5-4398B908CFD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28695" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Design</t>
   </si>
@@ -76,6 +76,33 @@
   </si>
   <si>
     <t>TO BE DECIDED: Spawn Position, random or markers?</t>
+  </si>
+  <si>
+    <t>Work On Design</t>
+  </si>
+  <si>
+    <t>Between Phases there will be a short cutscene</t>
+  </si>
+  <si>
+    <t>Create second Scene</t>
+  </si>
+  <si>
+    <t>Jumping Puzzle</t>
+  </si>
+  <si>
+    <t>Re-design-Boss</t>
+  </si>
+  <si>
+    <t>Add Orbs (same as first fight)</t>
+  </si>
+  <si>
+    <t>add Floor wipe mechanic</t>
+  </si>
+  <si>
+    <t>Work on the winning variables ()</t>
+  </si>
+  <si>
+    <t>still using the one from Level One</t>
   </si>
 </sst>
 </file>
@@ -405,15 +432,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B4:F18"/>
+  <dimension ref="B4:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="30.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="51.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -489,9 +516,52 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B18" t="s">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adds floating platform texture
</commit_message>
<xml_diff>
--- a/Documents/ToDo.xlsx
+++ b/Documents/ToDo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro\Desktop\PlayGround\Games\FirstPlatformer\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9548889B-0CEF-4B1A-86D5-4398B908CFD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{902BA58E-71D4-42A7-8AB8-309F99159DAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28695" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Design</t>
   </si>
@@ -99,10 +99,7 @@
     <t>add Floor wipe mechanic</t>
   </si>
   <si>
-    <t>Work on the winning variables ()</t>
-  </si>
-  <si>
-    <t>still using the one from Level One</t>
+    <t>Work on the winning/game Over variables ()</t>
   </si>
 </sst>
 </file>
@@ -435,7 +432,7 @@
   <dimension ref="B4:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -516,52 +513,49 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>24</v>
-      </c>
-      <c r="C28" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>